<commit_message>
Added files up to RD plot
</commit_message>
<xml_diff>
--- a/Library/Charts/Chart of marginal effect with results table using excel/figure.xlsx
+++ b/Library/Charts/Chart of marginal effect with results table using excel/figure.xlsx
@@ -238,49 +238,49 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="D3" s="1">
-        <v>0.1066666666666667</v>
+        <v>0.224</v>
       </c>
       <c r="E3" s="1">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="F3" s="1">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="G3" s="1">
-        <v>0.037383177570093497</v>
+        <v>0.15642458100558659</v>
       </c>
       <c r="H3" s="1">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="J3" s="1">
-        <v>0.27906976744186052</v>
+        <v>0.39436619718309862</v>
       </c>
       <c r="K3" s="1">
-        <v>7.4941713609147529</v>
+        <v>3.7390578596597623</v>
       </c>
       <c r="L3" s="1">
-        <v>4.5713291219920427</v>
+        <v>1.4685474569468147</v>
       </c>
       <c r="M3" s="1">
-        <v>3.3019285496909245</v>
+        <v>3.3578726911263548</v>
       </c>
       <c r="N3" s="1">
-        <v>0.00096022526679579833</v>
+        <v>0.00078544779410171666</v>
       </c>
       <c r="O3" s="1">
-        <v>2.2672728438228273</v>
+        <v>1.7315912590284546</v>
       </c>
       <c r="P3" s="1">
-        <v>24.770995047980044</v>
+        <v>8.0738185787144268</v>
       </c>
     </row>
     <row r="4">
@@ -288,49 +288,49 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1">
+        <v>250</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.056000000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>179</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.033519553072625698</v>
+      </c>
+      <c r="H4" s="1">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
-        <v>150</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.053333333333333302</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>107</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.0280373831775701</v>
-      </c>
-      <c r="H4" s="1">
-        <v>5</v>
-      </c>
       <c r="I4" s="1">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="J4" s="1">
-        <v>0.1162790697674419</v>
+        <v>0.1126760563380282</v>
       </c>
       <c r="K4" s="1">
-        <v>4.2401468218652445</v>
+        <v>3.5945943348961187</v>
       </c>
       <c r="L4" s="1">
-        <v>3.0157869478445263</v>
+        <v>2.0701756354350751</v>
       </c>
       <c r="M4" s="1">
-        <v>2.031080870567751</v>
+        <v>2.2215679969295099</v>
       </c>
       <c r="N4" s="1">
-        <v>0.042246791634581143</v>
+        <v>0.026312514671228783</v>
       </c>
       <c r="O4" s="1">
-        <v>1.051882685088138</v>
+        <v>1.1626028168804754</v>
       </c>
       <c r="P4" s="1">
-        <v>17.0920629513618</v>
+        <v>11.1139490158277</v>
       </c>
     </row>
     <row r="5">
@@ -391,46 +391,46 @@
         <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="D6" s="1">
-        <v>0.11</v>
+        <v>0.043999999999999997</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="G6" s="1">
-        <v>0.041666666666666699</v>
+        <v>0.0167597765363128</v>
       </c>
       <c r="H6" s="1">
         <v>8</v>
       </c>
       <c r="I6" s="1">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="J6" s="1">
-        <v>0.2857142857142857</v>
+        <v>0.1126760563380282</v>
       </c>
       <c r="K6" s="1">
-        <v>9.6086487418963369</v>
+        <v>8.7196803624762946</v>
       </c>
       <c r="L6" s="1">
-        <v>7.1306741634296893</v>
+        <v>6.3810709023567025</v>
       </c>
       <c r="M6" s="1">
-        <v>3.0489599284619917</v>
+        <v>2.9592506020988121</v>
       </c>
       <c r="N6" s="1">
-        <v>0.0022963510938419597</v>
+        <v>0.003083882065132851</v>
       </c>
       <c r="O6" s="1">
-        <v>2.2437638870344108</v>
+        <v>2.0777362438253051</v>
       </c>
       <c r="P6" s="1">
-        <v>41.147881547899303</v>
+        <v>36.594070036421584</v>
       </c>
     </row>
     <row r="7">

</xml_diff>